<commit_message>
Added UPdated Code Into Branch
</commit_message>
<xml_diff>
--- a/database/PRJ-005/literature/keywords.xlsx
+++ b/database/PRJ-005/literature/keywords.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iziel-my.sharepoint.com/personal/sachin_ghadage_izielhealthcare_com/Documents/Desktop/CEP-CER-AI/Testing/Zest-Microetcher/Literature-Screening/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iziel-my.sharepoint.com/personal/sachin_ghadage_izielhealthcare_com/Documents/Desktop/CEP-CER-AI/Testing/Spacelabs-BISx/Literature-Screening/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="11_161981FAF613C8264F2C4C65F59059496C0277F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3730061-CE07-4FF8-A015-C76D83684AA3}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_085D68DFD063D60E623554765836FE3B962B942A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FA7EB9B-82B1-47A5-9867-739CEE48BA5F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
   <si>
     <t>Keyword No.</t>
   </si>
@@ -34,124 +34,166 @@
     <t>Date Range</t>
   </si>
   <si>
-    <t>Unnamed: 4</t>
-  </si>
-  <si>
     <t>Number of Hits</t>
   </si>
   <si>
     <t>#1</t>
   </si>
   <si>
+    <t>("electroencephalogram" OR "EEG") AND ("Bispectral index" OR "BIS")</t>
+  </si>
+  <si>
+    <t>01 October 2024 to 30 September 2025</t>
+  </si>
+  <si>
+    <t>31.0, 31</t>
+  </si>
+  <si>
     <t>#2</t>
   </si>
   <si>
+    <t>"patient monitoring" AND ("anesthesia" OR "sedation")</t>
+  </si>
+  <si>
+    <t>23.0, 23</t>
+  </si>
+  <si>
     <t>#3</t>
   </si>
   <si>
+    <t>("anesthesia" OR "sedation") AND "EEG"</t>
+  </si>
+  <si>
+    <t>129.0, 129</t>
+  </si>
+  <si>
     <t>#4</t>
   </si>
   <si>
+    <t>("EEG" OR "EEG module" OR "electroencephalogram") AND "Patient Monitoring"</t>
+  </si>
+  <si>
+    <t>4.0, 4</t>
+  </si>
+  <si>
     <t>#5</t>
   </si>
   <si>
+    <t>"Bispectral index" AND "hospital" AND "monitors"</t>
+  </si>
+  <si>
+    <t>19.0, 19</t>
+  </si>
+  <si>
     <t>#6</t>
   </si>
   <si>
+    <t>("BIS" OR "Bispectral Index") AND "Philips"</t>
+  </si>
+  <si>
+    <t>2.0, 2</t>
+  </si>
+  <si>
     <t>#7</t>
   </si>
   <si>
+    <t>("E BIS" OR "Bispectral Index") AND "GE Healthcare"</t>
+  </si>
+  <si>
+    <t>1.0, 1</t>
+  </si>
+  <si>
     <t>#8</t>
   </si>
   <si>
+    <t>"6800-30-50486" AND "Mindray"</t>
+  </si>
+  <si>
+    <t>0.0, 0</t>
+  </si>
+  <si>
     <t>#9</t>
   </si>
   <si>
+    <t>"Spacelabs" AND "Bispectral index"</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
     <t>#10</t>
   </si>
   <si>
+    <t>"Spacelabs" AND "91482"</t>
+  </si>
+  <si>
     <t>#11</t>
   </si>
   <si>
+    <t>("Bispectral Index" OR "Bispectral Index Analysis Module") AND ("brain data acquisition" OR "EEG data acquisition" OR "acquisition of EEG signals" OR "incidence of awareness" OR "anesthetic administration" OR "general anesthesia" OR "sedation")</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
     <t>#12</t>
   </si>
   <si>
+    <t>("Bispectral Index") AND ("brain" OR "data acquisition" OR "EEG signals" OR "anesthetic agent")</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
     <t>#13</t>
   </si>
   <si>
+    <t>("Bispectral Index") AND ("no display" OR "loss of data" OR "no alarm" OR "injury") AND "risk"</t>
+  </si>
+  <si>
     <t>#14</t>
   </si>
   <si>
+    <t>("Bispectral Index") AND ("BISx Interface Cable" OR "BISx"</t>
+  </si>
+  <si>
     <t>#15</t>
   </si>
   <si>
+    <t>"BIS pod" OR "BIS Sensor"</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>#16</t>
   </si>
   <si>
+    <t>("Bispectral Index") AND ("real-time encephalogram" OR "real-time EEG") AND ("adults" AND "pediatrics")</t>
+  </si>
+  <si>
     <t>#17</t>
   </si>
   <si>
+    <t>("brain wave measurement" OR "brain wave frequency" OR "depth of consciousness") AND ("EEG" OR "BIS")</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>#18</t>
   </si>
   <si>
+    <t>("supression ratio" OR "Spectral Edge Frequency" OR "Median Power Frequency" OR "Electromyographic strength" OR "Signal Quality Index" OR "Burst Count") AND "BIS"</t>
+  </si>
+  <si>
     <t>#19</t>
   </si>
   <si>
-    <t>(("Sandblaster" OR "Air abrasion" OR "Intraoral Sandblaster") AND ( "bonding" OR "Bond strength") AND ("Aluminum Oxide"))</t>
-  </si>
-  <si>
-    <t>("Sandblaster" OR "Air abrasion" OR "Intraoral Sandblaster") AND (“cement removal” OR “Resin removal” OR “cleaning”)</t>
-  </si>
-  <si>
-    <t>((“SilJet” OR "CoJet Sand" OR "Rocatec Pre") AND (“Repair” OR "Pretreatment" OR "composite restorations" OR "restoration" OR Silane))</t>
-  </si>
-  <si>
-    <t>("Sandblaster" OR "Air abrasion" OR "Intraoral Sandblaster") AND ("glass beads")</t>
-  </si>
-  <si>
-    <t>("Sandblaster" OR "air abrasion") AND ("bond strength" OR "bonding")</t>
-  </si>
-  <si>
-    <t>("Air abrasion” OR "Sandblast") AND ("sensitivity" OR "Postoperative sensitivity")</t>
-  </si>
-  <si>
-    <t>(“Air abrasion” OR "Sandblast") AND ("retention")</t>
-  </si>
-  <si>
-    <t>("Air abrasion" OR "Sandblast") AND ("leakage" OR "microleakage" OR "Restoration" OR "patient comfort") </t>
-  </si>
-  <si>
-    <t>("sandblasting " OR "air abrasion") AND ("bonding" OR "surface preparation" OR "cement removal" OR "orthodontic bracket removal") AND ("aluminum oxide" OR "siljet" OR "sodium bicarbonate")</t>
-  </si>
-  <si>
-    <t>("intraoral sandblasting" OR " sandblaster" OR "air abrasion") AND ("porcelain repair" OR "composite repair" OR "denture repair" OR "pit and fissure " OR "surface conditioning " OR "surface roughening" )</t>
-  </si>
-  <si>
-    <t>("acid etching" OR "etching") AND ("surface preparation" OR "surface roughening" OR "bonding") </t>
-  </si>
-  <si>
-    <t>("Diamond bur" OR "Carbide") AND ("retention" OR "Restoration")</t>
-  </si>
-  <si>
-    <t>("self etching primer" OR "zirconia primer" OR "Pumice polishing") AND ("Bonding" OR "cleaning" OR "stain removal")</t>
-  </si>
-  <si>
-    <t>(("SA85" OR "micron" OR "aluminum oxide") AND ("enamel erosion"))</t>
-  </si>
-  <si>
-    <t>((“Microroughening” OR “MicroEtcher”) AND (“Zest Dental”))</t>
-  </si>
-  <si>
-    <t>("PrepStart" OR "AquaCare") AND ("Retention" OR "bond strength" OR "bonding" OR "patient comfort" OR "Stain removal")</t>
-  </si>
-  <si>
-    <t>"MicroEtcher" AND ("air abrasion" OR "micro abrasion" OR "intraoral sandblasting" OR "sandblasting") AND ("surface roughening" OR "cement removal" OR "porcelain repair" OR "composite repair" OR "orthodontic adhesive removal" OR "fissure preparation")</t>
-  </si>
-  <si>
-    <t>((“Sandblasting”) AND (“MicroEtcher” OR “Zest Dental”))</t>
-  </si>
-  <si>
-    <t>"MicroEtcher" AND ("Retention" OR "bond strength" OR "bonding" OR "patient comfort" OR "Stain removal")</t>
+    <t>("depth of consciousness" OR "sedation level") AND "BIS"</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -169,10 +211,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -233,9 +272,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -273,7 +312,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -307,7 +346,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -342,10 +380,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -522,12 +559,13 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="74" customWidth="1"/>
+    <col min="3" max="3" width="132.42578125" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -543,223 +581,245 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2">
-        <v>17</v>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3">
-        <v>12</v>
+      <c r="F3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6">
-        <v>44</v>
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
         <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9">
-        <v>16</v>
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="F11">
-        <v>8</v>
+      <c r="F11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12">
-        <v>408</v>
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14">
-        <v>16</v>
+        <v>42</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
+        <v>44</v>
+      </c>
+      <c r="F15" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="F17" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
+        <v>51</v>
+      </c>
+      <c r="F18" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
+        <v>54</v>
+      </c>
+      <c r="F19" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
+        <v>56</v>
+      </c>
+      <c r="F20" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>